<commit_message>
Update RS for MS-ASNOTE
</commit_message>
<xml_diff>
--- a/ExchangeActiveSync/Docs/MS-ASNOTE/MS-ASNOTE_RequirementSpecification.xlsx
+++ b/ExchangeActiveSync/Docs/MS-ASNOTE/MS-ASNOTE_RequirementSpecification.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB783CE-1EBB-4744-AF20-182EAC955C43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8860A875-7B2D-4AF6-889E-6B50E939CA8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2505" yWindow="1185" windowWidth="18570" windowHeight="11595" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2272" uniqueCount="388">
   <si>
     <t>Req ID</t>
   </si>
@@ -1234,21 +1234,6 @@
     <t>2.7.5</t>
   </si>
   <si>
-    <t>[In Body] Protocol version 14.0 supports this [In Body] element.</t>
-  </si>
-  <si>
-    <t>[In Body] Protocol version 14.1 supports this [In Body] element.</t>
-  </si>
-  <si>
-    <t>[In Body] Protocol version 16.0 supports this [In Body] element.</t>
-  </si>
-  <si>
-    <t>[In Body] Protocol version 16.1 supports this [In Body] element.</t>
-  </si>
-  <si>
-    <t>[In Body] Protocol version 12.1 does not supports this [In Body] element.</t>
-  </si>
-  <si>
     <t>MS-ASNOTE_R43001</t>
   </si>
   <si>
@@ -1264,21 +1249,6 @@
     <t>MS-ASNOTE_R43005</t>
   </si>
   <si>
-    <t>[In Category] Protocol version 12.1 does not supports this [In Category] element.</t>
-  </si>
-  <si>
-    <t>[In Category] Protocol version 14.0 supports this [In Category] element.</t>
-  </si>
-  <si>
-    <t>[In Category] Protocol version 14.1 supports this [In Category] element.</t>
-  </si>
-  <si>
-    <t>[In Category] Protocol version 16.0 supports this [In Category] element.</t>
-  </si>
-  <si>
-    <t>[In Category] Protocol version 16.1 supports this [In Category] element.</t>
-  </si>
-  <si>
     <t>MS-ASNOTE_R50001</t>
   </si>
   <si>
@@ -1327,63 +1297,6 @@
     <t>[In Subject] Protocol version 16.1 supports this [In Subject] element.</t>
   </si>
   <si>
-    <t>[In Subject] Protocol version 16.0 supports this [In Subject] element.</t>
-  </si>
-  <si>
-    <t>[In Subject] Protocol version 14.1 supports this [In Subject] element.</t>
-  </si>
-  <si>
-    <t>[In Subject] Protocol version 14.0 supports this [In Subject] element.</t>
-  </si>
-  <si>
-    <t>[In Subject] Protocol version 12.1 does not supports this [In Subject] element.</t>
-  </si>
-  <si>
-    <t>[In MessageClass] The Subject element specifies the subject of the note.</t>
-  </si>
-  <si>
-    <t>[In MessageClass] Protocol version 16.1 supports this [In MessageClass] element.</t>
-  </si>
-  <si>
-    <t>[In MessageClass] Protocol version 16.0 supports this [In MessageClass] element.</t>
-  </si>
-  <si>
-    <t>[In MessageClass] Protocol version 14.1 supports this [In MessageClass] element.</t>
-  </si>
-  <si>
-    <t>[In MessageClass] Protocol version 14.0 supports this [In MessageClass] element.</t>
-  </si>
-  <si>
-    <t>[In MessageClass] Protocol version 12.1 does not supports this [In MessageClass] element.</t>
-  </si>
-  <si>
-    <t>MS-ASNOTE_R58001</t>
-  </si>
-  <si>
-    <t>MS-ASNOTE_R58002</t>
-  </si>
-  <si>
-    <t>MS-ASNOTE_R58003</t>
-  </si>
-  <si>
-    <t>MS-ASNOTE_R58004</t>
-  </si>
-  <si>
-    <t>MS-ASNOTE_R58005</t>
-  </si>
-  <si>
-    <t>[In LastModifiedDate] Protocol version 16.1 supports this [In LastModifiedDate] element.</t>
-  </si>
-  <si>
-    <t>[In LastModifiedDate] Protocol version 16.0 supports this [In LastModifiedDate] element.</t>
-  </si>
-  <si>
-    <t>[In LastModifiedDate] Protocol version 14.1 supports this [In LastModifiedDate] element.</t>
-  </si>
-  <si>
-    <t>[In LastModifiedDate] Protocol version 14.0 supports this [In LastModifiedDate] element.</t>
-  </si>
-  <si>
     <t>MS-ASNOTE_R53001</t>
   </si>
   <si>
@@ -1399,22 +1312,112 @@
     <t>MS-ASNOTE_R53005</t>
   </si>
   <si>
-    <t>[In LastModifiedDate] Protocol version 12.1 does not supports this [In LastModifiedDate] element.</t>
-  </si>
-  <si>
-    <t>[In Categories] Protocol version 12.1 does not supports this [In Categories] element.</t>
-  </si>
-  <si>
-    <t>[In Categories] Protocol version 14.0 supports this [In Categories] element.</t>
-  </si>
-  <si>
-    <t>[In Categories] Protocol version 14.1 supports this [In Categories] element.</t>
-  </si>
-  <si>
-    <t>[In Categories] Protocol version 16.0 supports this [In Categories] element.</t>
-  </si>
-  <si>
-    <t>[In Categories] Protocol version 16.1 supports this [In Categories] element.</t>
+    <t>[In Subject] The Subject element specifies the subject of the note.</t>
+  </si>
+  <si>
+    <t>MS-ASNOTE_R57001</t>
+  </si>
+  <si>
+    <t>MS-ASNOTE_R57002</t>
+  </si>
+  <si>
+    <t>MS-ASNOTE_R57003</t>
+  </si>
+  <si>
+    <t>MS-ASNOTE_R57004</t>
+  </si>
+  <si>
+    <t>MS-ASNOTE_R57005</t>
+  </si>
+  <si>
+    <t>[In Body] Protocol version 12.1 does not supports this [Body] element.</t>
+  </si>
+  <si>
+    <t>[In Body] Protocol version 14.0 supports this [Body] element.</t>
+  </si>
+  <si>
+    <t>[In Body] Protocol version 14.1 supports this [Body] element.</t>
+  </si>
+  <si>
+    <t>[In Body] Protocol version 16.0 supports this [Body] element.</t>
+  </si>
+  <si>
+    <t>[In Body] Protocol version 16.1 supports this [Body] element.</t>
+  </si>
+  <si>
+    <t>[In Categories] Protocol version 12.1 does not supports this [Categories] element.</t>
+  </si>
+  <si>
+    <t>[In Categories] Protocol version 14.0 supports this [Categories] element.</t>
+  </si>
+  <si>
+    <t>[In Categories] Protocol version 14.1 supports this [Categories] element.</t>
+  </si>
+  <si>
+    <t>[In Categories] Protocol version 16.0 supports this [Categories] element.</t>
+  </si>
+  <si>
+    <t>[In Categories] Protocol version 16.1 supports this [Categories] element.</t>
+  </si>
+  <si>
+    <t>[In Category] Protocol version 12.1 does not supports this [Category] element.</t>
+  </si>
+  <si>
+    <t>[In Category] Protocol version 14.0 supports this [Category] element.</t>
+  </si>
+  <si>
+    <t>[In Category] Protocol version 14.1 supports this [Category] element.</t>
+  </si>
+  <si>
+    <t>[In Category] Protocol version 16.0 supports this [Category] element.</t>
+  </si>
+  <si>
+    <t>[In Category] Protocol version 16.1 supports this [Category] element.</t>
+  </si>
+  <si>
+    <t>[In LastModifiedDate] Protocol version 14.0 supports this [LastModifiedDate] element.</t>
+  </si>
+  <si>
+    <t>[In LastModifiedDate] Protocol version 14.1 supports this [LastModifiedDate] element.</t>
+  </si>
+  <si>
+    <t>[In LastModifiedDate] Protocol version 16.0 supports this [LastModifiedDate] element.</t>
+  </si>
+  <si>
+    <t>[In LastModifiedDate] Protocol version 16.1 supports this [LastModifiedDate] element.</t>
+  </si>
+  <si>
+    <t>[In LastModifiedDate] Protocol version 12.1 does not supports this [LastModifiedDate] element.</t>
+  </si>
+  <si>
+    <t>[In MessageClass] Protocol version 12.1 does not supports this [MessageClass] element.</t>
+  </si>
+  <si>
+    <t>[In MessageClass] Protocol version 14.0 supports this [MessageClass] element.</t>
+  </si>
+  <si>
+    <t>[In MessageClass] Protocol version 14.1 supports this [MessageClass] element.</t>
+  </si>
+  <si>
+    <t>[In MessageClass] Protocol version 16.0 supports this [MessageClass] element.</t>
+  </si>
+  <si>
+    <t>[In MessageClass] Protocol version 16.1 supports this [MessageClass] element.</t>
+  </si>
+  <si>
+    <t>[In Subject] Protocol version 12.1 does not supports this [Subject] element.</t>
+  </si>
+  <si>
+    <t>[In Subject] Protocol version 14.0 supports this [Subject] element.</t>
+  </si>
+  <si>
+    <t>[In Subject] Protocol version 14.1 supports this [ubject] element.</t>
+  </si>
+  <si>
+    <t>[In Subject] Protocol version 16.0 supports this [Subject] element.</t>
+  </si>
+  <si>
+    <t>[In Subject] Protocol version 16.1 supports this [Subject] element.</t>
   </si>
 </sst>
 </file>
@@ -1693,21 +1696,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1732,191 +1720,26 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="137">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="143">
     <dxf>
       <fill>
         <patternFill>
@@ -2292,6 +2115,216 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.59996337778862885"/>
@@ -2333,179 +2366,6 @@
     <dxf>
       <font>
         <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
       </font>
     </dxf>
     <dxf>
@@ -2669,6 +2529,179 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
@@ -2802,34 +2835,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I175" tableType="xml" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I175" tableType="xml" totalsRowShown="0" headerRowDxfId="142" dataDxfId="141" connectionId="1">
   <autoFilter ref="A19:I175" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="126">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="140">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="125">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="139">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="124">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="138">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="123">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="137">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="122">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="136">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="121">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="135">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="120">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="134">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="119">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="133">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="118">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="132">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -2838,12 +2871,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="136" dataDxfId="134" headerRowBorderDxfId="135" tableBorderDxfId="133" totalsRowBorderDxfId="132">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="131" dataDxfId="129" headerRowBorderDxfId="130" tableBorderDxfId="128" totalsRowBorderDxfId="127">
   <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="131"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="130"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="129"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="126"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="125"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="124"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3173,8 +3206,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3231,128 +3264,128 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -3365,12 +3398,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -3383,12 +3416,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -3401,12 +3434,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -3419,60 +3452,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -4407,13 +4440,13 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="22" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B56" s="24" t="s">
         <v>173</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>330</v>
+        <v>358</v>
       </c>
       <c r="D56" s="30"/>
       <c r="E56" s="30" t="s">
@@ -4432,13 +4465,13 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="22" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B57" s="24" t="s">
         <v>173</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>326</v>
+        <v>359</v>
       </c>
       <c r="D57" s="30"/>
       <c r="E57" s="30" t="s">
@@ -4457,13 +4490,13 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="22" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B58" s="24" t="s">
         <v>173</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>327</v>
+        <v>360</v>
       </c>
       <c r="D58" s="30"/>
       <c r="E58" s="30" t="s">
@@ -4482,13 +4515,13 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="22" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B59" s="24" t="s">
         <v>173</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>328</v>
+        <v>361</v>
       </c>
       <c r="D59" s="30"/>
       <c r="E59" s="30" t="s">
@@ -4507,13 +4540,13 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="22" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="B60" s="24" t="s">
         <v>173</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>329</v>
+        <v>362</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30" t="s">
@@ -4607,13 +4640,13 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="22" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="B64" s="31" t="s">
         <v>174</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>382</v>
+        <v>363</v>
       </c>
       <c r="D64" s="30"/>
       <c r="E64" s="30" t="s">
@@ -4632,13 +4665,13 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="22" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="B65" s="31" t="s">
         <v>174</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>383</v>
+        <v>364</v>
       </c>
       <c r="D65" s="30"/>
       <c r="E65" s="30" t="s">
@@ -4657,13 +4690,13 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="22" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="B66" s="31" t="s">
         <v>174</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>384</v>
+        <v>365</v>
       </c>
       <c r="D66" s="30"/>
       <c r="E66" s="30" t="s">
@@ -4682,13 +4715,13 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="22" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="B67" s="31" t="s">
         <v>174</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>385</v>
+        <v>366</v>
       </c>
       <c r="D67" s="30"/>
       <c r="E67" s="30" t="s">
@@ -4707,13 +4740,13 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="22" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="B68" s="31" t="s">
         <v>174</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>386</v>
+        <v>367</v>
       </c>
       <c r="D68" s="30"/>
       <c r="E68" s="30" t="s">
@@ -4832,13 +4865,13 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="22" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="B73" s="31" t="s">
         <v>175</v>
       </c>
       <c r="C73" s="21" t="s">
-        <v>336</v>
+        <v>368</v>
       </c>
       <c r="D73" s="30"/>
       <c r="E73" s="30" t="s">
@@ -4857,13 +4890,13 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="22" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="B74" s="31" t="s">
         <v>175</v>
       </c>
       <c r="C74" s="21" t="s">
-        <v>337</v>
+        <v>369</v>
       </c>
       <c r="D74" s="30"/>
       <c r="E74" s="30" t="s">
@@ -4882,13 +4915,13 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="22" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="B75" s="31" t="s">
         <v>175</v>
       </c>
       <c r="C75" s="21" t="s">
-        <v>338</v>
+        <v>370</v>
       </c>
       <c r="D75" s="30"/>
       <c r="E75" s="30" t="s">
@@ -4907,13 +4940,13 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="22" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="B76" s="31" t="s">
         <v>175</v>
       </c>
       <c r="C76" s="21" t="s">
-        <v>339</v>
+        <v>371</v>
       </c>
       <c r="D76" s="30"/>
       <c r="E76" s="30" t="s">
@@ -4932,13 +4965,13 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="22" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="B77" s="31" t="s">
         <v>175</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>340</v>
+        <v>372</v>
       </c>
       <c r="D77" s="30"/>
       <c r="E77" s="30" t="s">
@@ -5032,13 +5065,13 @@
     </row>
     <row r="81" spans="1:9" ht="30">
       <c r="A81" s="22" t="s">
-        <v>376</v>
+        <v>347</v>
       </c>
       <c r="B81" s="31" t="s">
         <v>176</v>
       </c>
       <c r="C81" s="21" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D81" s="30"/>
       <c r="E81" s="30" t="s">
@@ -5057,13 +5090,13 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="22" t="s">
-        <v>377</v>
+        <v>348</v>
       </c>
       <c r="B82" s="31" t="s">
         <v>176</v>
       </c>
       <c r="C82" s="21" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D82" s="30"/>
       <c r="E82" s="30" t="s">
@@ -5082,7 +5115,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="22" t="s">
-        <v>378</v>
+        <v>349</v>
       </c>
       <c r="B83" s="31" t="s">
         <v>176</v>
@@ -5107,13 +5140,13 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="22" t="s">
-        <v>379</v>
+        <v>350</v>
       </c>
       <c r="B84" s="31" t="s">
         <v>176</v>
       </c>
       <c r="C84" s="21" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D84" s="30"/>
       <c r="E84" s="30" t="s">
@@ -5132,13 +5165,13 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="22" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="B85" s="31" t="s">
         <v>176</v>
       </c>
       <c r="C85" s="21" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="D85" s="30"/>
       <c r="E85" s="30" t="s">
@@ -5256,14 +5289,14 @@
       <c r="I89" s="32"/>
     </row>
     <row r="90" spans="1:9">
-      <c r="A90" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="B90" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="C90" s="20" t="s">
-        <v>361</v>
+      <c r="A90" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="B90" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="C90" s="21" t="s">
+        <v>378</v>
       </c>
       <c r="D90" s="30"/>
       <c r="E90" s="30" t="s">
@@ -5276,19 +5309,19 @@
         <v>15</v>
       </c>
       <c r="H90" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I90" s="32"/>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="22" t="s">
-        <v>367</v>
-      </c>
-      <c r="B91" s="31" t="s">
-        <v>178</v>
+        <v>354</v>
+      </c>
+      <c r="B91" s="24" t="s">
+        <v>177</v>
       </c>
       <c r="C91" s="21" t="s">
-        <v>366</v>
+        <v>379</v>
       </c>
       <c r="D91" s="30"/>
       <c r="E91" s="30" t="s">
@@ -5307,13 +5340,13 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="22" t="s">
-        <v>368</v>
-      </c>
-      <c r="B92" s="31" t="s">
-        <v>178</v>
+        <v>355</v>
+      </c>
+      <c r="B92" s="24" t="s">
+        <v>177</v>
       </c>
       <c r="C92" s="21" t="s">
-        <v>365</v>
+        <v>380</v>
       </c>
       <c r="D92" s="30"/>
       <c r="E92" s="30" t="s">
@@ -5332,13 +5365,13 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="22" t="s">
-        <v>369</v>
-      </c>
-      <c r="B93" s="31" t="s">
-        <v>178</v>
+        <v>356</v>
+      </c>
+      <c r="B93" s="24" t="s">
+        <v>177</v>
       </c>
       <c r="C93" s="21" t="s">
-        <v>364</v>
+        <v>381</v>
       </c>
       <c r="D93" s="30"/>
       <c r="E93" s="30" t="s">
@@ -5357,13 +5390,13 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="22" t="s">
-        <v>370</v>
-      </c>
-      <c r="B94" s="31" t="s">
-        <v>178</v>
+        <v>357</v>
+      </c>
+      <c r="B94" s="24" t="s">
+        <v>177</v>
       </c>
       <c r="C94" s="21" t="s">
-        <v>363</v>
+        <v>382</v>
       </c>
       <c r="D94" s="30"/>
       <c r="E94" s="30" t="s">
@@ -5381,14 +5414,14 @@
       <c r="I94" s="32"/>
     </row>
     <row r="95" spans="1:9">
-      <c r="A95" s="22" t="s">
-        <v>371</v>
-      </c>
-      <c r="B95" s="31" t="s">
+      <c r="A95" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B95" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="C95" s="21" t="s">
-        <v>362</v>
+      <c r="C95" s="20" t="s">
+        <v>352</v>
       </c>
       <c r="D95" s="30"/>
       <c r="E95" s="30" t="s">
@@ -5401,7 +5434,7 @@
         <v>15</v>
       </c>
       <c r="H95" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I95" s="32"/>
     </row>
@@ -5457,13 +5490,13 @@
     </row>
     <row r="98" spans="1:9">
       <c r="A98" s="22" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="B98" s="31" t="s">
         <v>178</v>
       </c>
       <c r="C98" s="21" t="s">
-        <v>360</v>
+        <v>383</v>
       </c>
       <c r="D98" s="30"/>
       <c r="E98" s="30" t="s">
@@ -5482,13 +5515,13 @@
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="22" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B99" s="31" t="s">
         <v>178</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>359</v>
+        <v>384</v>
       </c>
       <c r="D99" s="30"/>
       <c r="E99" s="30" t="s">
@@ -5507,13 +5540,13 @@
     </row>
     <row r="100" spans="1:9">
       <c r="A100" s="22" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B100" s="31" t="s">
         <v>178</v>
       </c>
       <c r="C100" s="21" t="s">
-        <v>358</v>
+        <v>385</v>
       </c>
       <c r="D100" s="30"/>
       <c r="E100" s="30" t="s">
@@ -5532,13 +5565,13 @@
     </row>
     <row r="101" spans="1:9">
       <c r="A101" s="22" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B101" s="31" t="s">
         <v>178</v>
       </c>
       <c r="C101" s="21" t="s">
-        <v>357</v>
+        <v>386</v>
       </c>
       <c r="D101" s="30"/>
       <c r="E101" s="30" t="s">
@@ -5557,13 +5590,13 @@
     </row>
     <row r="102" spans="1:9">
       <c r="A102" s="22" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B102" s="31" t="s">
         <v>178</v>
       </c>
       <c r="C102" s="21" t="s">
-        <v>356</v>
+        <v>387</v>
       </c>
       <c r="D102" s="30"/>
       <c r="E102" s="30" t="s">
@@ -7415,6 +7448,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -7422,297 +7460,314 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I20:I89 A20:H55 A34:I55 A61:I63 D56:I60 A56:B60 A78:I80 A73:B77 D73:I77 A69:I72 A64:B68 D64:I68 A86:I89 D91:D95 A103:I175 A98:B102 D98:I102 A96:I97 I91:I158 H91:I95 A81:B85 D81:I85">
-    <cfRule type="expression" dxfId="117" priority="163">
+  <conditionalFormatting sqref="I20:I89 A20:H55 A34:I55 A61:I63 D56:I60 A56:B60 A78:I80 A73:B77 D73:I77 A69:I72 A64:B68 D64:I68 A86:I89 D90:D94 A103:I175 A98:B102 D98:I102 A96:I97 H90:I94 A81:B85 D81:I85 I96:I158">
+    <cfRule type="expression" dxfId="123" priority="171">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="164">
+    <cfRule type="expression" dxfId="122" priority="172">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="171">
+    <cfRule type="expression" dxfId="121" priority="179">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:I89 A20:H55 A34:I55 A61:I63 D56:I60 A56:B60 A78:I80 A73:B77 D73:I77 A69:I72 A64:B68 D64:I68 A86:I89 D91:D95 A103:I175 A98:B102 D98:I102 A96:I97 I91:I158 H91:I95 A81:B85 D81:I85">
-    <cfRule type="expression" dxfId="114" priority="117">
+  <conditionalFormatting sqref="I20:I89 A20:H55 A34:I55 A61:I63 D56:I60 A56:B60 A78:I80 A73:B77 D73:I77 A69:I72 A64:B68 D64:I68 A86:I89 D90:D94 A103:I175 A98:B102 D98:I102 A96:I97 H90:I94 A81:B85 D81:I85 I96:I158">
+    <cfRule type="expression" dxfId="120" priority="125">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="118">
+    <cfRule type="expression" dxfId="119" priority="126">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="119">
+    <cfRule type="expression" dxfId="118" priority="127">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F96:F175 F20:F89">
-    <cfRule type="expression" dxfId="111" priority="123">
+  <conditionalFormatting sqref="F96:F175 F20:F94">
+    <cfRule type="expression" dxfId="117" priority="131">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="124">
+    <cfRule type="expression" dxfId="116" priority="132">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C59">
-    <cfRule type="expression" dxfId="109" priority="108">
+    <cfRule type="expression" dxfId="115" priority="116">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="109">
+    <cfRule type="expression" dxfId="114" priority="117">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="110">
+    <cfRule type="expression" dxfId="113" priority="118">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C59">
-    <cfRule type="expression" dxfId="106" priority="105">
+    <cfRule type="expression" dxfId="112" priority="113">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="106">
+    <cfRule type="expression" dxfId="111" priority="114">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="107">
+    <cfRule type="expression" dxfId="110" priority="115">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="103" priority="102">
+    <cfRule type="expression" dxfId="109" priority="110">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="103">
+    <cfRule type="expression" dxfId="108" priority="111">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="104">
+    <cfRule type="expression" dxfId="107" priority="112">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="100" priority="99">
+    <cfRule type="expression" dxfId="106" priority="107">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="100">
+    <cfRule type="expression" dxfId="105" priority="108">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="101">
+    <cfRule type="expression" dxfId="104" priority="109">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C73:C76">
-    <cfRule type="expression" dxfId="97" priority="96">
+    <cfRule type="expression" dxfId="103" priority="104">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="97">
+    <cfRule type="expression" dxfId="102" priority="105">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="98">
+    <cfRule type="expression" dxfId="101" priority="106">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C73:C76">
-    <cfRule type="expression" dxfId="94" priority="93">
+    <cfRule type="expression" dxfId="100" priority="101">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="94">
+    <cfRule type="expression" dxfId="99" priority="102">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="95">
+    <cfRule type="expression" dxfId="98" priority="103">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
-    <cfRule type="expression" dxfId="91" priority="90">
+    <cfRule type="expression" dxfId="97" priority="98">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="91">
+    <cfRule type="expression" dxfId="96" priority="99">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="92">
+    <cfRule type="expression" dxfId="95" priority="100">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
-    <cfRule type="expression" dxfId="88" priority="87">
+    <cfRule type="expression" dxfId="94" priority="95">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="88">
+    <cfRule type="expression" dxfId="93" priority="96">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="89">
+    <cfRule type="expression" dxfId="92" priority="97">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:C67">
-    <cfRule type="expression" dxfId="85" priority="84">
+    <cfRule type="expression" dxfId="91" priority="92">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="85">
+    <cfRule type="expression" dxfId="90" priority="93">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="86">
+    <cfRule type="expression" dxfId="89" priority="94">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:C67">
-    <cfRule type="expression" dxfId="82" priority="81">
+    <cfRule type="expression" dxfId="88" priority="89">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="82">
+    <cfRule type="expression" dxfId="87" priority="90">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="83">
+    <cfRule type="expression" dxfId="86" priority="91">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68">
-    <cfRule type="expression" dxfId="79" priority="78">
+    <cfRule type="expression" dxfId="85" priority="86">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="79">
+    <cfRule type="expression" dxfId="84" priority="87">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="80">
+    <cfRule type="expression" dxfId="83" priority="88">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68">
-    <cfRule type="expression" dxfId="76" priority="75">
+    <cfRule type="expression" dxfId="82" priority="83">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="76">
+    <cfRule type="expression" dxfId="81" priority="84">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="77">
+    <cfRule type="expression" dxfId="80" priority="85">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C84">
-    <cfRule type="expression" dxfId="73" priority="72">
+    <cfRule type="expression" dxfId="79" priority="80">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="73">
+    <cfRule type="expression" dxfId="78" priority="81">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="74">
+    <cfRule type="expression" dxfId="77" priority="82">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C84">
-    <cfRule type="expression" dxfId="70" priority="69">
+    <cfRule type="expression" dxfId="76" priority="77">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="70">
+    <cfRule type="expression" dxfId="75" priority="78">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="71">
+    <cfRule type="expression" dxfId="74" priority="79">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C85">
-    <cfRule type="expression" dxfId="67" priority="66">
+    <cfRule type="expression" dxfId="73" priority="74">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="67">
+    <cfRule type="expression" dxfId="72" priority="75">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="68">
+    <cfRule type="expression" dxfId="71" priority="76">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C85">
-    <cfRule type="expression" dxfId="64" priority="63">
+    <cfRule type="expression" dxfId="70" priority="71">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="64">
+    <cfRule type="expression" dxfId="69" priority="72">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="65">
+    <cfRule type="expression" dxfId="68" priority="73">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C91:C94">
-    <cfRule type="expression" dxfId="61" priority="60">
+  <conditionalFormatting sqref="C90:C93">
+    <cfRule type="expression" dxfId="67" priority="68">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="61">
+    <cfRule type="expression" dxfId="66" priority="69">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="62">
+    <cfRule type="expression" dxfId="65" priority="70">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C91:C94">
-    <cfRule type="expression" dxfId="58" priority="57">
+  <conditionalFormatting sqref="C90:C93">
+    <cfRule type="expression" dxfId="64" priority="65">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="58">
+    <cfRule type="expression" dxfId="63" priority="66">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="59">
+    <cfRule type="expression" dxfId="62" priority="67">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C95">
-    <cfRule type="expression" dxfId="55" priority="54">
+  <conditionalFormatting sqref="C94">
+    <cfRule type="expression" dxfId="61" priority="62">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="55">
+    <cfRule type="expression" dxfId="60" priority="63">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="56">
+    <cfRule type="expression" dxfId="59" priority="64">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C95">
-    <cfRule type="expression" dxfId="52" priority="51">
+  <conditionalFormatting sqref="C94">
+    <cfRule type="expression" dxfId="58" priority="59">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="52">
+    <cfRule type="expression" dxfId="57" priority="60">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="53">
+    <cfRule type="expression" dxfId="56" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98:C101">
-    <cfRule type="expression" dxfId="49" priority="48">
+    <cfRule type="expression" dxfId="55" priority="56">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="49">
+    <cfRule type="expression" dxfId="54" priority="57">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="50">
+    <cfRule type="expression" dxfId="53" priority="58">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98:C101">
-    <cfRule type="expression" dxfId="46" priority="45">
+    <cfRule type="expression" dxfId="52" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="46">
+    <cfRule type="expression" dxfId="51" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="47">
+    <cfRule type="expression" dxfId="50" priority="55">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C102">
-    <cfRule type="expression" dxfId="43" priority="42">
+    <cfRule type="expression" dxfId="49" priority="50">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="43">
+    <cfRule type="expression" dxfId="48" priority="51">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="44">
+    <cfRule type="expression" dxfId="47" priority="52">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C102">
+    <cfRule type="expression" dxfId="46" priority="47">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="48">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="49">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90:A94 E90:G94">
+    <cfRule type="expression" dxfId="43" priority="44">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="45">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="46">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90:A94 E90:G94">
     <cfRule type="expression" dxfId="40" priority="39">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -7723,144 +7778,144 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A90:I90 A91:A95 E91:G95">
-    <cfRule type="expression" dxfId="35" priority="36">
+  <conditionalFormatting sqref="B90">
+    <cfRule type="expression" dxfId="37" priority="36">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="37">
+    <cfRule type="expression" dxfId="36" priority="37">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="38">
+    <cfRule type="expression" dxfId="35" priority="38">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A90:I90 A91:A95 E91:G95">
-    <cfRule type="expression" dxfId="32" priority="31">
+  <conditionalFormatting sqref="B90">
+    <cfRule type="expression" dxfId="34" priority="33">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="32">
+    <cfRule type="expression" dxfId="33" priority="34">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="33">
+    <cfRule type="expression" dxfId="32" priority="35">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F90:F95">
-    <cfRule type="expression" dxfId="37" priority="34">
-      <formula>NOT(VLOOKUP(F90,$A$12:$C$15,2,FALSE)="In")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="35">
-      <formula>(VLOOKUP(F90,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" dxfId="29" priority="28">
+    <cfRule type="expression" dxfId="31" priority="30">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="29">
+    <cfRule type="expression" dxfId="30" priority="31">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="30">
+    <cfRule type="expression" dxfId="29" priority="32">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" dxfId="26" priority="25">
+    <cfRule type="expression" dxfId="28" priority="27">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="26">
+    <cfRule type="expression" dxfId="27" priority="28">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="27">
+    <cfRule type="expression" dxfId="26" priority="29">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="expression" dxfId="23" priority="22">
+    <cfRule type="expression" dxfId="25" priority="24">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="23">
+    <cfRule type="expression" dxfId="24" priority="25">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="24">
+    <cfRule type="expression" dxfId="23" priority="26">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="expression" dxfId="20" priority="19">
+    <cfRule type="expression" dxfId="22" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="21" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="21">
+    <cfRule type="expression" dxfId="20" priority="23">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="expression" dxfId="17" priority="16">
+    <cfRule type="expression" dxfId="19" priority="18">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="18">
+    <cfRule type="expression" dxfId="17" priority="20">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="16" priority="15">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="14" priority="17">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="13" priority="12">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="11" priority="14">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="10" priority="9">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="8" priority="11">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B95">
-    <cfRule type="expression" dxfId="5" priority="4">
+  <conditionalFormatting sqref="A95:I95">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B95">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="A95:I95">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F95">
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>NOT(VLOOKUP(F95,$A$12:$C$15,2,FALSE)="In")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="5">
+      <formula>(VLOOKUP(F95,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
@@ -7903,15 +7958,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -7960,6 +8006,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
@@ -7975,14 +8030,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7995,4 +8042,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>